<commit_message>
New "weird" plot + gene_data update
</commit_message>
<xml_diff>
--- a/data/gene_data.xlsx
+++ b/data/gene_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BunBun\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\mar\Dev\Projects\R\Vasc-AoP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985BD26D-697D-4848-90B9-57BF0D28F1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329FFF3A-F89C-441F-9C74-D296BF4952E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7980" yWindow="825" windowWidth="20355" windowHeight="12015" activeTab="1" xr2:uid="{79E2ED8E-6715-464F-B0D9-EF27996045FB}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="1" xr2:uid="{79E2ED8E-6715-464F-B0D9-EF27996045FB}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="1" r:id="rId1"/>
@@ -110,9 +110,6 @@
     <t>Extracellular Matrix</t>
   </si>
   <si>
-    <t>Pathway_family</t>
-  </si>
-  <si>
     <t>Gene_name</t>
   </si>
   <si>
@@ -428,9 +425,6 @@
     <t>10.1016/j.brainres.2018.03.012; 10.3171/jns.2005.103.1.0136; 10.1161/01.STR.0000170712.46106.2e</t>
   </si>
   <si>
-    <t>Function</t>
-  </si>
-  <si>
     <t>Vascular stabilization and maturation</t>
   </si>
   <si>
@@ -461,9 +455,6 @@
     <t>Flt1; Tie1</t>
   </si>
   <si>
-    <t>Tgfb1; Flk1; Angpt1, Tek; Vegfa</t>
-  </si>
-  <si>
     <t>Cdh5; Vegfa; Mmp2; Mmp9; Angpt2</t>
   </si>
   <si>
@@ -477,6 +468,15 @@
   </si>
   <si>
     <t>Lect1; Angpt2; Thbs1; Serpinf1</t>
+  </si>
+  <si>
+    <t>Tgfb1; Flk1; Angpt1; Tek; Vegfa</t>
+  </si>
+  <si>
+    <t>Effect</t>
+  </si>
+  <si>
+    <t>Fx</t>
   </si>
 </sst>
 </file>
@@ -589,7 +589,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{549967FE-54FA-4134-AF28-96D3DFB2641F}"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{50EA19DA-04A9-4AE2-939A-F27CB5D5588A}"/>
@@ -613,7 +613,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -912,587 +912,587 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C24"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="60.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.15234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.15234375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.15234375" customWidth="1"/>
     <col min="6" max="6" width="164" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>145</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" t="s">
         <v>89</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B2" t="s">
-        <v>90</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G13" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" t="s">
         <v>97</v>
       </c>
-      <c r="E15" t="s">
-        <v>98</v>
-      </c>
       <c r="F15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G17" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D20" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" t="s">
+        <v>126</v>
+      </c>
+      <c r="F20" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A21" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" t="s">
+        <v>101</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F21" t="s">
+        <v>57</v>
+      </c>
+      <c r="G21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A22" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="E20" t="s">
-        <v>127</v>
-      </c>
-      <c r="F20" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B21" t="s">
-        <v>90</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="D21" t="s">
-        <v>102</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F21" t="s">
-        <v>58</v>
-      </c>
-      <c r="G21" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G22" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G23" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G24" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>108</v>
-      </c>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>111</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1515,88 +1515,88 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="9" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
         <v>133</v>
       </c>
-      <c r="B4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>134</v>
-      </c>
-      <c r="B5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>135</v>
-      </c>
       <c r="B6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>21</v>

</xml_diff>